<commit_message>
karma karp running time tex file
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -71,11 +71,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -90,6 +91,12 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="6.4"/>
+      <color rgb="FF3C3C3C"/>
+      <name val="Ubuntu"/>
       <family val="0"/>
     </font>
   </fonts>
@@ -135,8 +142,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -149,6 +160,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF3C3C3C"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -157,15 +228,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T53"/>
+  <dimension ref="A1:T143"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A53" activeCellId="0" sqref="A53"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A42" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B55" activeCellId="0" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2468,6 +2539,543 @@
       <c r="T53" s="0" t="n">
         <f aca="false">AVERAGE(T2:T51)</f>
         <v>2.2358600854876</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B55" s="1" t="n">
+        <f aca="false">FREQUENCY($A$2:$A$51,$A$55:$A$143)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="n">
+        <f aca="false">A55+10000</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="n">
+        <f aca="false">A56+20000</f>
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="n">
+        <f aca="false">A57+20000</f>
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="n">
+        <f aca="false">A58+20000</f>
+        <v>70000</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="n">
+        <f aca="false">A59+20000</f>
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="n">
+        <f aca="false">A60+20000</f>
+        <v>110000</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="n">
+        <f aca="false">A61+20000</f>
+        <v>130000</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="n">
+        <f aca="false">A62+20000</f>
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="n">
+        <f aca="false">A63+20000</f>
+        <v>170000</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="n">
+        <f aca="false">A64+20000</f>
+        <v>190000</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="n">
+        <f aca="false">A65+20000</f>
+        <v>210000</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="n">
+        <f aca="false">A66+20000</f>
+        <v>230000</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="n">
+        <f aca="false">A67+20000</f>
+        <v>250000</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="n">
+        <f aca="false">A68+20000</f>
+        <v>270000</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="n">
+        <f aca="false">A69+20000</f>
+        <v>290000</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="n">
+        <f aca="false">A70+20000</f>
+        <v>310000</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="n">
+        <f aca="false">A71+20000</f>
+        <v>330000</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="n">
+        <f aca="false">A72+20000</f>
+        <v>350000</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="n">
+        <f aca="false">A73+20000</f>
+        <v>370000</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="n">
+        <f aca="false">A74+20000</f>
+        <v>390000</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="n">
+        <f aca="false">A75+20000</f>
+        <v>410000</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="n">
+        <f aca="false">A76+20000</f>
+        <v>430000</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="n">
+        <f aca="false">A77+20000</f>
+        <v>450000</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="n">
+        <f aca="false">A78+20000</f>
+        <v>470000</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="n">
+        <f aca="false">A79+20000</f>
+        <v>490000</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="n">
+        <f aca="false">A80+20000</f>
+        <v>510000</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="n">
+        <f aca="false">A81+20000</f>
+        <v>530000</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="n">
+        <f aca="false">A82+20000</f>
+        <v>550000</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="n">
+        <f aca="false">A83+20000</f>
+        <v>570000</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="n">
+        <f aca="false">A84+20000</f>
+        <v>590000</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="n">
+        <f aca="false">A85+20000</f>
+        <v>610000</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="n">
+        <f aca="false">A86+20000</f>
+        <v>630000</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="n">
+        <f aca="false">A87+20000</f>
+        <v>650000</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="n">
+        <f aca="false">A88+20000</f>
+        <v>670000</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="n">
+        <f aca="false">A89+20000</f>
+        <v>690000</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="n">
+        <f aca="false">A90+20000</f>
+        <v>710000</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="n">
+        <f aca="false">A91+20000</f>
+        <v>730000</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="n">
+        <f aca="false">A92+20000</f>
+        <v>750000</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="n">
+        <f aca="false">A93+20000</f>
+        <v>770000</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="n">
+        <f aca="false">A94+20000</f>
+        <v>790000</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="n">
+        <f aca="false">A95+20000</f>
+        <v>810000</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="n">
+        <f aca="false">A96+20000</f>
+        <v>830000</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="n">
+        <f aca="false">A97+20000</f>
+        <v>850000</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="n">
+        <f aca="false">A98+20000</f>
+        <v>870000</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="n">
+        <f aca="false">A99+20000</f>
+        <v>890000</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="n">
+        <f aca="false">A100+20000</f>
+        <v>910000</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="n">
+        <f aca="false">A101+20000</f>
+        <v>930000</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="n">
+        <f aca="false">A102+20000</f>
+        <v>950000</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="n">
+        <f aca="false">A103+20000</f>
+        <v>970000</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="n">
+        <f aca="false">A104+20000</f>
+        <v>990000</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="n">
+        <f aca="false">A105+20000</f>
+        <v>1010000</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="n">
+        <f aca="false">A106+20000</f>
+        <v>1030000</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="n">
+        <f aca="false">A107+20000</f>
+        <v>1050000</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="n">
+        <f aca="false">A108+20000</f>
+        <v>1070000</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="n">
+        <f aca="false">A109+20000</f>
+        <v>1090000</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="0" t="n">
+        <f aca="false">A110+20000</f>
+        <v>1110000</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="n">
+        <f aca="false">A111+20000</f>
+        <v>1130000</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="0" t="n">
+        <f aca="false">A112+20000</f>
+        <v>1150000</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="n">
+        <f aca="false">A113+20000</f>
+        <v>1170000</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="n">
+        <f aca="false">A114+20000</f>
+        <v>1190000</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="n">
+        <f aca="false">A115+20000</f>
+        <v>1210000</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="n">
+        <f aca="false">A116+20000</f>
+        <v>1230000</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="n">
+        <f aca="false">A117+20000</f>
+        <v>1250000</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="n">
+        <f aca="false">A118+20000</f>
+        <v>1270000</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="n">
+        <f aca="false">A119+20000</f>
+        <v>1290000</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="n">
+        <f aca="false">A120+20000</f>
+        <v>1310000</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="n">
+        <f aca="false">A121+20000</f>
+        <v>1330000</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="n">
+        <f aca="false">A122+20000</f>
+        <v>1350000</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="0" t="n">
+        <f aca="false">A123+20000</f>
+        <v>1370000</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="0" t="n">
+        <f aca="false">A124+20000</f>
+        <v>1390000</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="0" t="n">
+        <f aca="false">A125+20000</f>
+        <v>1410000</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="0" t="n">
+        <f aca="false">A126+20000</f>
+        <v>1430000</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="0" t="n">
+        <f aca="false">A127+20000</f>
+        <v>1450000</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="0" t="n">
+        <f aca="false">A128+20000</f>
+        <v>1470000</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="0" t="n">
+        <f aca="false">A129+20000</f>
+        <v>1490000</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="0" t="n">
+        <f aca="false">A130+20000</f>
+        <v>1510000</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="0" t="n">
+        <f aca="false">A131+20000</f>
+        <v>1530000</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="0" t="n">
+        <f aca="false">A132+20000</f>
+        <v>1550000</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="0" t="n">
+        <f aca="false">A133+20000</f>
+        <v>1570000</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="0" t="n">
+        <f aca="false">A134+20000</f>
+        <v>1590000</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="0" t="n">
+        <f aca="false">A135+20000</f>
+        <v>1610000</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="0" t="n">
+        <f aca="false">A136+20000</f>
+        <v>1630000</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="0" t="n">
+        <f aca="false">A137+20000</f>
+        <v>1650000</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="0" t="n">
+        <f aca="false">A138+20000</f>
+        <v>1670000</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="0" t="n">
+        <f aca="false">A139+20000</f>
+        <v>1690000</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="0" t="n">
+        <f aca="false">A140+20000</f>
+        <v>1710000</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="0" t="n">
+        <f aca="false">A141+20000</f>
+        <v>1730000</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="0" t="n">
+        <f aca="false">A142+20000</f>
+        <v>1750000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>